<commit_message>
main player enter scene
</commit_message>
<xml_diff>
--- a/rawconfig/map.xlsx
+++ b/rawconfig/map.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="scene" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="116">
   <si>
     <t>array</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -426,6 +426,34 @@
   </si>
   <si>
     <t>skill</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>初始位置x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>初始位置y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>初始位置z</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pos_x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pos_y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pos_z</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -772,10 +800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -784,7 +812,7 @@
     <col min="5" max="5" width="13.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -800,8 +828,17 @@
       <c r="E1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -814,8 +851,17 @@
       <c r="E2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -831,8 +877,17 @@
       <c r="E3" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G3" t="s">
+        <v>114</v>
+      </c>
+      <c r="H3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -848,8 +903,17 @@
       <c r="E4" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B5">
         <v>100000</v>
       </c>
@@ -862,8 +926,17 @@
       <c r="E5">
         <v>100000</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F5">
+        <v>2628</v>
+      </c>
+      <c r="G5">
+        <v>9</v>
+      </c>
+      <c r="H5">
+        <v>1891</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B6">
         <v>100001</v>
       </c>
@@ -876,8 +949,17 @@
       <c r="E6">
         <v>100000</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F6">
+        <v>2628</v>
+      </c>
+      <c r="G6">
+        <v>9</v>
+      </c>
+      <c r="H6">
+        <v>1891</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B7">
         <v>100002</v>
       </c>
@@ -890,8 +972,17 @@
       <c r="E7">
         <v>100000</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F7">
+        <v>2628</v>
+      </c>
+      <c r="G7">
+        <v>9</v>
+      </c>
+      <c r="H7">
+        <v>1891</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B8">
         <v>100003</v>
       </c>
@@ -904,8 +995,17 @@
       <c r="E8">
         <v>100000</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F8">
+        <v>2628</v>
+      </c>
+      <c r="G8">
+        <v>9</v>
+      </c>
+      <c r="H8">
+        <v>1891</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B9">
         <v>100004</v>
       </c>
@@ -918,8 +1018,17 @@
       <c r="E9">
         <v>100000</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F9">
+        <v>2628</v>
+      </c>
+      <c r="G9">
+        <v>9</v>
+      </c>
+      <c r="H9">
+        <v>1891</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B10">
         <v>100005</v>
       </c>
@@ -931,6 +1040,15 @@
       </c>
       <c r="E10">
         <v>100000</v>
+      </c>
+      <c r="F10">
+        <v>2628</v>
+      </c>
+      <c r="G10">
+        <v>9</v>
+      </c>
+      <c r="H10">
+        <v>1891</v>
       </c>
     </row>
   </sheetData>
@@ -944,8 +1062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="U12" sqref="U12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Z1" sqref="Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>